<commit_message>
filled up some of the report sections
</commit_message>
<xml_diff>
--- a/report/Book1.xlsx
+++ b/report/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Method</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Baseline [8]</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -210,12 +213,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="35830784"/>
-        <c:axId val="35980032"/>
+        <c:axId val="162606464"/>
+        <c:axId val="162624640"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="35830784"/>
+        <c:axId val="162606464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -224,7 +227,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="35980032"/>
+        <c:crossAx val="162624640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -232,7 +235,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35980032"/>
+        <c:axId val="162624640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -243,7 +246,155 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="35830784"/>
+        <c:crossAx val="162606464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="36725120"/>
+        <c:axId val="36726656"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="36725120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="36726656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="36726656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="36725120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -264,16 +415,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1457325</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2381250</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -287,6 +438,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1409700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -582,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D1" sqref="D1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +775,7 @@
     <col min="2" max="2" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,8 +785,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -615,8 +799,11 @@
       <c r="C2">
         <v>18945.931339999999</v>
       </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -626,8 +813,11 @@
       <c r="C3">
         <v>19800.99899</v>
       </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -637,8 +827,11 @@
       <c r="C4">
         <v>19953.011490000001</v>
       </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -648,8 +841,11 @@
       <c r="C5">
         <v>20201.641019999999</v>
       </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -659,8 +855,11 @@
       <c r="C6">
         <v>20525.75794</v>
       </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -670,8 +869,11 @@
       <c r="C7">
         <v>20560.675230000001</v>
       </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -681,8 +883,11 @@
       <c r="C8">
         <v>21634.16113</v>
       </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -691,6 +896,9 @@
       </c>
       <c r="C9">
         <v>25572.582979999999</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>